<commit_message>
Adding the Testcases guid and did code cleanup
</commit_message>
<xml_diff>
--- a/oneMap/TestData/OneMap_TestData.xlsx
+++ b/oneMap/TestData/OneMap_TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>TestName</t>
   </si>
@@ -24,15 +24,9 @@
     <t>SearchKeyWord</t>
   </si>
   <si>
-    <t>performKeywordSearch_TC_001</t>
-  </si>
-  <si>
     <t>Marina Mall</t>
   </si>
   <si>
-    <t>performKeywordSearch_TC_002</t>
-  </si>
-  <si>
     <t>PostalCode</t>
   </si>
   <si>
@@ -51,19 +45,31 @@
     <t>Destination2</t>
   </si>
   <si>
-    <t>verifyRouteToDestination1_TC_001</t>
-  </si>
-  <si>
     <t>SourceLocation</t>
   </si>
   <si>
-    <t>verifyRouteToDestination2_TC_002</t>
-  </si>
-  <si>
     <t>598751</t>
   </si>
   <si>
     <t>FARRER PARK MRT</t>
+  </si>
+  <si>
+    <t>JURONG EAST</t>
+  </si>
+  <si>
+    <t>verifyPostalCodeSearch_TC_002</t>
+  </si>
+  <si>
+    <t>verifyKeywordSearch_TC_001</t>
+  </si>
+  <si>
+    <t>verifyRouteToDestination1_TC_003</t>
+  </si>
+  <si>
+    <t>verifyRouteToDestination2_TC_004</t>
+  </si>
+  <si>
+    <t>verifySwitchDestination_TC_005</t>
   </si>
 </sst>
 </file>
@@ -411,7 +417,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -429,26 +435,26 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -459,15 +465,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.26953125" customWidth="1"/>
+    <col min="1" max="1" width="37.54296875" customWidth="1"/>
     <col min="2" max="2" width="29.54296875" customWidth="1"/>
     <col min="3" max="3" width="27.7265625" customWidth="1"/>
     <col min="4" max="4" width="28.6328125" customWidth="1"/>
@@ -478,38 +484,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>